<commit_message>
play out xlsx to json conversion
</commit_message>
<xml_diff>
--- a/JsonPlay/chords.xlsx
+++ b/JsonPlay/chords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sandbox\git\aadennis\PythonSandboxAA\JsonPlay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sandbox\git\aadennis\PythonSandboxAA\JsonPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B3B747-71D1-474E-935C-BAD1F7FAF096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92C89B5-4136-4502-92B6-2B7432222B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0A32EA1-7CCB-4C83-95EC-DFA7D8184C5D}"/>
+    <workbookView xWindow="-25728" yWindow="5088" windowWidth="21300" windowHeight="11880" xr2:uid="{D0A32EA1-7CCB-4C83-95EC-DFA7D8184C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>c_pf</t>
   </si>
@@ -50,24 +50,15 @@
     <t>name</t>
   </si>
   <si>
-    <t>key</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>C Major</t>
   </si>
   <si>
     <t>E3</t>
   </si>
   <si>
-    <t>c_mi</t>
-  </si>
-  <si>
     <t>C Minor</t>
   </si>
   <si>
@@ -93,13 +84,112 @@
   </si>
   <si>
     <t>c_sus4</t>
+  </si>
+  <si>
+    <t>D#3</t>
+  </si>
+  <si>
+    <t>C sus2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>C sus4</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>c_maj</t>
+  </si>
+  <si>
+    <t>tested</t>
+  </si>
+  <si>
+    <t>c_min</t>
+  </si>
+  <si>
+    <t>c_add2</t>
+  </si>
+  <si>
+    <t>c_add4</t>
+  </si>
+  <si>
+    <t>C add2</t>
+  </si>
+  <si>
+    <t>C add4</t>
+  </si>
+  <si>
+    <t>c_aug</t>
+  </si>
+  <si>
+    <t>C aug</t>
+  </si>
+  <si>
+    <t>G#3</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A#2</t>
+  </si>
+  <si>
+    <t>c_dim</t>
+  </si>
+  <si>
+    <t>C dim</t>
+  </si>
+  <si>
+    <t>F#3</t>
+  </si>
+  <si>
+    <t>c_6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A#3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>only the root is played</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>key2</t>
+  </si>
+  <si>
+    <t>key3</t>
+  </si>
+  <si>
+    <t>key4</t>
+  </si>
+  <si>
+    <t>key5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,13 +197,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,8 +237,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,123 +584,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEF97C8-4EBD-4E32-A042-1320C503EEC4}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
columns added to chord data
</commit_message>
<xml_diff>
--- a/JsonPlay/chords.xlsx
+++ b/JsonPlay/chords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sandbox\git\aadennis\PythonSandboxAA\JsonPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92C89B5-4136-4502-92B6-2B7432222B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45711731-BB3F-4719-B96A-50AB1DD5E910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25728" yWindow="5088" windowWidth="21300" windowHeight="11880" xr2:uid="{D0A32EA1-7CCB-4C83-95EC-DFA7D8184C5D}"/>
   </bookViews>
@@ -587,7 +587,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>